<commit_message>
Modifiche varie alla documentazione
</commit_message>
<xml_diff>
--- a/Documentation/CPS-ASV-Q&A.xlsx
+++ b/Documentation/CPS-ASV-Q&A.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Questions</t>
   </si>
@@ -34,11 +34,21 @@
     <t xml:space="preserve">Android Version on phone</t>
   </si>
   <si>
-    <t xml:space="preserve">Android 5+
+    <t xml:space="preserve">Nexus 5X
+Android 6.0
+minimum SDK 21, preferrably SDK 23 or higher
+Fake_GPS
+Build Number: MDA89E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android version on tablet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FireHD_IO(5th_Generation) Amazon
+S.O: FireOS 5.3.3.0
+Samsung GTP51110
+S.O: CyanoGenMod Android 6.0.1
 minimum SDK 21, preferrably SDK 23 or higher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android version on tablet</t>
   </si>
   <si>
     <t xml:space="preserve">Communication protocol between tablet and smart-phone</t>
@@ -66,6 +76,9 @@
 Have also used Ubiquiti Rocket on the shore when we have larger teams of boats.</t>
   </si>
   <si>
+    <t xml:space="preserve">Router Vulnerabilities Default Configuration: https://www.sec-consult.com/fxdata/seccons/prod/temedia/advisories_txt/20151105-0_Ubiquiti_Networks_Insecure_Default_Configuration_v10.txt </t>
+  </si>
+  <si>
     <t xml:space="preserve">Communication protocol between phone and Arduino</t>
   </si>
   <si>
@@ -114,8 +127,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -214,28 +228,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -317,132 +331,138 @@
   </sheetPr>
   <dimension ref="A1:Z65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.3163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="120.086734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="84.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="57.9387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="65.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="192.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="4" customFormat="false" ht="243.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="5" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>14</v>
+      <c r="A8" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>16</v>
+      <c r="A9" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" display="https://www.sec-consult.com/fxdata/seccons/prod/temedia/advisories_txt/20151105-0_Ubiquiti_Networks_Insecure_Default_Configuration_v10.txt"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>